<commit_message>
path rettet og packagename
</commit_message>
<xml_diff>
--- a/src/main/resources/files/Suppliers_by_Spend.xlsx
+++ b/src/main/resources/files/Suppliers_by_Spend.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
   <si>
     <t>Name</t>
   </si>
@@ -26,48 +26,6 @@
   </si>
   <si>
     <t>Volume €</t>
-  </si>
-  <si>
-    <t>Computer Store</t>
-  </si>
-  <si>
-    <t>Nokia</t>
-  </si>
-  <si>
-    <t>DataStore</t>
-  </si>
-  <si>
-    <t>DataStoreUusi</t>
-  </si>
-  <si>
-    <t>kiva</t>
-  </si>
-  <si>
-    <t>Fiji</t>
-  </si>
-  <si>
-    <t>Afghanistan</t>
-  </si>
-  <si>
-    <t>Belize</t>
-  </si>
-  <si>
-    <t>Laptops</t>
-  </si>
-  <si>
-    <t>Accessories</t>
-  </si>
-  <si>
-    <t>Laptops, Mobile Phones</t>
-  </si>
-  <si>
-    <t>Accessories, Laptops, Mobile Phones, Printers, Screens</t>
-  </si>
-  <si>
-    <t>hhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhhh</t>
-  </si>
-  <si>
-    <t>Printers</t>
   </si>
 </sst>
 </file>
@@ -136,9 +94,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="15.19921875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.65625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="49.8671875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="6.3359375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="8.265625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="18.234375" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="9.7421875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -154,76 +112,6 @@
       </c>
       <c r="D1" t="s" s="1">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.0</v>
       </c>
     </row>
   </sheetData>
@@ -272,8 +160,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="108.36328125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="11.65625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="6.3359375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="8.265625" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="18.234375" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="9.7421875" customWidth="true" bestFit="true"/>
   </cols>
@@ -292,20 +180,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="n">
-        <v>30001.0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>